<commit_message>
PCF bug fixed as .r should have been put after bracket. Most warnings fixed
</commit_message>
<xml_diff>
--- a/GraphicsAssignment/Project Logbook - Jonathan Walsh.xlsx
+++ b/GraphicsAssignment/Project Logbook - Jonathan Walsh.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University\Y3\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FastUniversity\Project - DOUBLE\ProjectUmbra\GraphicsAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BAED22-57A8-4184-BB1B-F6B62D50576B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF0ADA4-8899-4481-945A-6BFE8D23E503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3633285-B9BE-426B-9417-877568C48A86}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -81,13 +81,16 @@
     <t xml:space="preserve">Get shadows working; 'Attempt' to Implement PCF shadows; </t>
   </si>
   <si>
-    <t>Got shadows working.  Tried to implement PCF but still have the aliasing.</t>
-  </si>
-  <si>
-    <t>Get PCF properly working; Implement other types of light, directional and maybe area for example; Find assets for scene</t>
-  </si>
-  <si>
     <t>Code looks messy. May cause confusion in the future. Solution: Add comments, get rid of literals, add classes, methods etc.</t>
+  </si>
+  <si>
+    <t>Got shadows working.  Implemented PCF shadows</t>
+  </si>
+  <si>
+    <t>When having multiple lights make sure the are in groups of 4.  For example 1 float4 or a float3 and float etc.  Try fixing as many warnings as possible as later on it would be harder to debug if these warnings are in the way too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Get arrays working for lights being passed over to shader.  Try fixing as many as the directx warnings as possible.  Improve program architecture further to make programming more generic.  Extra: Get assets together and setup the scene with the assets</t>
   </si>
 </sst>
 </file>
@@ -615,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7390414C-51CC-44A8-9B89-0B4F4774D093}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,16 +692,16 @@
     </row>
     <row r="4" spans="1:8" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>43780</v>
+        <v>43788</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="14">
         <v>7</v>
@@ -706,15 +709,17 @@
       <c r="F4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>43787</v>
+        <v>43795</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="12"/>
@@ -725,7 +730,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>43794</v>
+        <v>43802</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
@@ -737,7 +742,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>43801</v>
+        <v>43809</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
@@ -749,7 +754,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>43808</v>
+        <v>43816</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
@@ -760,9 +765,7 @@
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>43815</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="12"/>

</xml_diff>

<commit_message>
Got rid of render target warning. Got assets working and context as member var
</commit_message>
<xml_diff>
--- a/GraphicsAssignment/Project Logbook - Jonathan Walsh.xlsx
+++ b/GraphicsAssignment/Project Logbook - Jonathan Walsh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FastUniversity\Project - DOUBLE\ProjectUmbra\GraphicsAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF0ADA4-8899-4481-945A-6BFE8D23E503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EA574F-070D-41F6-A1AE-9481EA0725F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3633285-B9BE-426B-9417-877568C48A86}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Get arrays working for lights being passed over to shader.  Try fixing as many as the directx warnings as possible.  Improve program architecture further to make programming more generic.  Extra: Get assets together and setup the scene with the assets</t>
+  </si>
+  <si>
+    <t>Didn't get all warnings fixed and didn't improve architecture but got array of lights working</t>
+  </si>
+  <si>
+    <t>Supervisor advised going through code line by line to find where warnings coming from.  Could be something to do with something not being set up correctly for the first model.</t>
+  </si>
+  <si>
+    <t>Get all warnings fixed. Have member variable for device context in scene class as Get calls have an overhead. Start getting assets together</t>
+  </si>
+  <si>
+    <t>Have a scene setup with house and lamps. Extra: implement variance mapping</t>
   </si>
 </sst>
 </file>
@@ -619,7 +631,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,18 +733,26 @@
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="D5" s="12"/>
-      <c r="E5" s="14"/>
+      <c r="E5" s="14">
+        <v>6</v>
+      </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43802</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="C6" s="13"/>
       <c r="D6" s="12"/>
       <c r="E6" s="14"/>
@@ -740,11 +760,13 @@
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>43809</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="C7" s="13"/>
       <c r="D7" s="12"/>
       <c r="E7" s="14"/>

</xml_diff>